<commit_message>
added upodates to illumina automation
</commit_message>
<xml_diff>
--- a/database/FINAL_SRA.xlsx
+++ b/database/FINAL_SRA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u7119530/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u7119530/gadi_mount/ausarg/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394035EB-6D0A-C640-8512-24A3E40096E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457853E7-7476-3841-8C2A-0920F19189E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="308">
   <si>
     <t>Instructions:</t>
   </si>
@@ -1340,6 +1340,27 @@
   </si>
   <si>
     <t>/g/data/xl04/bpadata/Tiliqua_rugosa/raw/illumina/rnaseq/350827_AusARG_UNSW_HK5GJDRXY_CCAGGCACCA-TAATTAGCGT_S4_L002_R1_001.fastq.gz;/g/data/xl04/bpadata/Tiliqua_rugosa/raw/illumina/rnaseq/350827_AusARG_UNSW_HK5GJDRXY_CCAGGCACCA-TAATTAGCGT_S4_L002_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Bassiana duperreyi</t>
+  </si>
+  <si>
+    <t>/g/data/xl04/bpadata/Bassiana_duperreyi/raw/illumina/dnaseq/350747_AusARG_UNSW_HTYH7DRXX_GTATTCCACC-TTGTCTACAT_S2_L001_R1_001.fastq.gz;/g/data/xl04/bpadata/Bassiana_duperreyi/raw/illumina/dnaseq/350747_AusARG_UNSW_HTYH7DRXX_GTATTCCACC-TTGTCTACAT_S2_L001_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>BASDUE</t>
+  </si>
+  <si>
+    <t>/g/data/xl04/bpadata/Bassiana_duperreyi/raw/illumina/dnaseq/350747_AusARG_UNSW_HTYH7DRXX_GTATTCCACC-TTGTCTACAT_S2_L002_R1_001.fastq.gz;/g/data/xl04/bpadata/Bassiana_duperreyi/raw/illumina/dnaseq/350747_AusARG_UNSW_HTYH7DRXX_GTATTCCACC-TTGTCTACAT_S2_L002_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Pogona vitticeps</t>
+  </si>
+  <si>
+    <t>/g/data/xl04/bpadata/Pogona_vitticeps/raw/illumina/dnaseq/Pogona_combined_ILM.1.fastq.gz;/g/data/xl04/bpadata/Pogona_vitticeps/raw/illumina/dnaseq/Pogona_combined_ILM.2.fastq.gz</t>
+  </si>
+  <si>
+    <t>POGVIE</t>
   </si>
 </sst>
 </file>
@@ -1830,13 +1851,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2610,8 +2631,8 @@
   <dimension ref="A1:S286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G23" sqref="G23"/>
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3723,31 +3744,112 @@
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="K29" s="11"/>
+      <c r="B29" s="9">
+        <v>350747</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="R29" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="S29" s="13" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="K30" s="11"/>
+      <c r="B30" s="9">
+        <v>350747</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="R30" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="S30" s="13" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="K31" s="11"/>
+      <c r="C31" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="S31" s="13" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D32" s="11"/>
@@ -6115,8 +6217,8 @@
       <c r="A2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -6443,8 +6545,8 @@
       <c r="A39" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="45"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="44"/>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="29" t="s">
@@ -6527,7 +6629,7 @@
       <c r="A50" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="43"/>
+      <c r="B50" s="45"/>
       <c r="C50" s="42"/>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -7124,12 +7226,51 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -7142,51 +7283,12 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>